<commit_message>
Working on performance table table
</commit_message>
<xml_diff>
--- a/PerformanceTable.xlsx
+++ b/PerformanceTable.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Project Files\N-Body\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Project Files\N-Body\Parallel-N-Body\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55C1A892-BA0C-42F2-8BD5-CD0A049DBA5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B955ACD6-7C46-4608-BC4D-3A8C5B606042}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{7E97CE3A-31D6-4C49-8965-2B1756764954}"/>
   </bookViews>
@@ -456,7 +456,7 @@
       <name val="Montserrat"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -493,6 +493,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFB948"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -506,11 +512,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -518,9 +521,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -544,6 +544,27 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -552,14 +573,14 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF9E00"/>
+      <color rgb="FFFFB948"/>
+      <color rgb="FFFFE4B8"/>
       <color rgb="FFFFD48D"/>
-      <color rgb="FFFF9E00"/>
+      <color rgb="FFFFC361"/>
       <color rgb="FFFFBB4C"/>
       <color rgb="FFFFBD52"/>
       <color rgb="FFFFC76B"/>
-      <color rgb="FFFFC361"/>
-      <color rgb="FFFFE4B8"/>
-      <color rgb="FFFFB948"/>
       <color rgb="FF7B2CBF"/>
       <color rgb="FF3C096C"/>
     </mruColors>
@@ -579,7 +600,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>371475</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>61912</xdr:rowOff>
@@ -932,887 +953,1171 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F223BCBC-CBAE-4527-A091-6FBDA7E5C4E9}">
-  <dimension ref="A1:T25"/>
+  <dimension ref="A1:X25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="3.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11" style="2" customWidth="1"/>
-    <col min="5" max="5" width="3.7109375" style="2" customWidth="1"/>
-    <col min="6" max="20" width="12.28515625" style="2" customWidth="1"/>
-    <col min="21" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="8.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="3.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11" style="1" customWidth="1"/>
+    <col min="5" max="5" width="3.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="1.5703125" style="1" customWidth="1"/>
+    <col min="7" max="10" width="12.28515625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="1" style="1" customWidth="1"/>
+    <col min="12" max="15" width="12.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="1.140625" style="1" customWidth="1"/>
+    <col min="17" max="20" width="12.28515625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="1.28515625" style="1" customWidth="1"/>
+    <col min="22" max="24" width="12.28515625" style="1" customWidth="1"/>
+    <col min="25" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:24" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-    </row>
-    <row r="2" spans="1:20" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+    </row>
+    <row r="2" spans="1:24" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="6"/>
+      <c r="G2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="H2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="I2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="J2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="K2" s="7"/>
+      <c r="L2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="10" t="s">
+      <c r="M2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="N2" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="10" t="s">
+      <c r="O2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="N2" s="11" t="s">
+      <c r="P2" s="8"/>
+      <c r="Q2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="O2" s="11" t="s">
+      <c r="R2" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="P2" s="11" t="s">
+      <c r="S2" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="Q2" s="11" t="s">
+      <c r="T2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="R2" s="12" t="s">
+      <c r="U2" s="9"/>
+      <c r="V2" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="S2" s="12" t="s">
+      <c r="W2" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="T2" s="12" t="s">
+      <c r="X2" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>2</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>1500</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>2</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="2"/>
+      <c r="G3" s="4">
         <v>1388.8100999999999</v>
       </c>
-      <c r="G3" s="6">
+      <c r="H3" s="4">
         <v>1377.66815</v>
       </c>
-      <c r="H3" s="7">
+      <c r="I3" s="5">
         <v>1230.5202999999999</v>
       </c>
-      <c r="I3" s="6">
-        <f>MIN(F3:H3)</f>
+      <c r="J3" s="4">
+        <f>MIN(G3:I3)</f>
         <v>1230.5202999999999</v>
       </c>
-      <c r="J3" s="6">
+      <c r="K3" s="4"/>
+      <c r="L3" s="4">
         <v>733.85709999999995</v>
       </c>
-      <c r="K3" s="6">
+      <c r="M3" s="4">
         <v>765.85815000000002</v>
       </c>
-      <c r="L3" s="7">
+      <c r="N3" s="5">
         <v>703.28035</v>
       </c>
-      <c r="M3" s="6">
-        <f xml:space="preserve"> MIN(J3:L3)</f>
+      <c r="O3" s="4">
+        <f xml:space="preserve"> MIN(L3:N3)</f>
         <v>703.28035</v>
       </c>
-      <c r="N3" s="6">
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4">
         <v>1.89</v>
       </c>
-      <c r="O3" s="6">
+      <c r="R3" s="4">
         <v>1.79</v>
       </c>
-      <c r="P3" s="6">
+      <c r="S3" s="4">
         <v>1.74</v>
       </c>
-      <c r="Q3" s="6">
-        <f>MAX(N3:P3)</f>
+      <c r="T3" s="4">
+        <f>MAX(Q3:S3)</f>
         <v>1.89</v>
       </c>
-      <c r="R3" s="6">
+      <c r="U3" s="4"/>
+      <c r="V3" s="4">
         <v>0.94</v>
       </c>
-      <c r="S3" s="6">
+      <c r="W3" s="4">
         <v>0.89</v>
       </c>
-      <c r="T3" s="6">
+      <c r="X3" s="4">
         <v>0.87</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3">
-        <v>3</v>
-      </c>
-      <c r="C4" s="3" t="s">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6">
+      <c r="D4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4">
         <v>727.31280000000004</v>
       </c>
-      <c r="K4" s="6">
+      <c r="M4" s="4">
         <v>677.45740000000001</v>
       </c>
-      <c r="L4" s="7">
+      <c r="N4" s="5">
         <v>525.87789999999995</v>
       </c>
-      <c r="M4" s="6">
-        <f t="shared" ref="M4:M7" si="0" xml:space="preserve"> MIN(J4:L4)</f>
+      <c r="O4" s="4">
+        <f t="shared" ref="O4:O7" si="0" xml:space="preserve"> MIN(L4:N4)</f>
         <v>525.87789999999995</v>
       </c>
-      <c r="N4" s="6">
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4">
         <v>1.9</v>
       </c>
-      <c r="O4" s="6">
+      <c r="R4" s="4">
         <v>2.0299999999999998</v>
       </c>
-      <c r="P4" s="6">
+      <c r="S4" s="4">
         <v>2.33</v>
       </c>
-      <c r="Q4" s="6">
-        <f t="shared" ref="Q4:Q7" si="1">MAX(N4:P4)</f>
+      <c r="T4" s="4">
+        <f>MAX(Q4:S4)</f>
         <v>2.33</v>
       </c>
-      <c r="R4" s="6">
+      <c r="U4" s="4"/>
+      <c r="V4" s="4">
         <v>0.63</v>
       </c>
-      <c r="S4" s="6">
+      <c r="W4" s="4">
         <v>0.67</v>
       </c>
-      <c r="T4" s="6">
+      <c r="X4" s="4">
         <v>0.77</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
         <v>4</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6">
+      <c r="D5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4">
         <v>649.66800000000001</v>
       </c>
-      <c r="K5" s="6">
+      <c r="M5" s="4">
         <v>671.83939999999996</v>
       </c>
-      <c r="L5" s="7">
+      <c r="N5" s="5">
         <v>458.17910000000001</v>
       </c>
-      <c r="M5" s="6">
+      <c r="O5" s="4">
         <f t="shared" si="0"/>
         <v>458.17910000000001</v>
       </c>
-      <c r="N5" s="6">
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4">
         <v>2.13</v>
       </c>
-      <c r="O5" s="6">
+      <c r="R5" s="4">
         <v>2.0499999999999998</v>
       </c>
-      <c r="P5" s="6">
+      <c r="S5" s="4">
         <v>2.68</v>
       </c>
-      <c r="Q5" s="6">
-        <f t="shared" si="1"/>
+      <c r="T5" s="4">
+        <f>MAX(Q5:S5)</f>
         <v>2.68</v>
       </c>
-      <c r="R5" s="6">
+      <c r="U5" s="4"/>
+      <c r="V5" s="4">
         <v>0.53</v>
       </c>
-      <c r="S5" s="6">
+      <c r="W5" s="4">
         <v>0.51</v>
       </c>
-      <c r="T5" s="6">
+      <c r="X5" s="4">
         <v>0.67</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="3">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2">
         <v>5</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6">
+      <c r="D6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4">
         <v>630.76580000000001</v>
       </c>
-      <c r="K6" s="6">
+      <c r="M6" s="4">
         <v>646.03629999999998</v>
       </c>
-      <c r="L6" s="7">
+      <c r="N6" s="5">
         <v>445.25364999999999</v>
       </c>
-      <c r="M6" s="6">
+      <c r="O6" s="4">
         <f t="shared" si="0"/>
         <v>445.25364999999999</v>
       </c>
-      <c r="N6" s="6">
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4">
         <v>2.2000000000000002</v>
       </c>
-      <c r="O6" s="6">
+      <c r="R6" s="4">
         <v>2.13</v>
       </c>
-      <c r="P6" s="6">
+      <c r="S6" s="4">
         <v>2.76</v>
       </c>
-      <c r="Q6" s="6">
-        <f t="shared" si="1"/>
+      <c r="T6" s="4">
+        <f>MAX(Q6:S6)</f>
         <v>2.76</v>
       </c>
-      <c r="R6" s="6">
+      <c r="U6" s="4"/>
+      <c r="V6" s="4">
         <v>0.44</v>
       </c>
-      <c r="S6" s="6">
+      <c r="W6" s="4">
         <v>0.42</v>
       </c>
-      <c r="T6" s="6">
+      <c r="X6" s="4">
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="2">
         <v>6</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6">
+      <c r="D7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4">
         <v>595.91875000000005</v>
       </c>
-      <c r="K7" s="6">
+      <c r="M7" s="4">
         <v>578.61159999999995</v>
       </c>
-      <c r="L7" s="7">
+      <c r="N7" s="5">
         <v>409.6515</v>
       </c>
-      <c r="M7" s="6">
+      <c r="O7" s="4">
         <f t="shared" si="0"/>
         <v>409.6515</v>
       </c>
-      <c r="N7" s="6">
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4">
         <v>2.33</v>
       </c>
-      <c r="O7" s="6">
+      <c r="R7" s="4">
         <v>2.38</v>
       </c>
-      <c r="P7" s="6">
-        <v>3</v>
-      </c>
-      <c r="Q7" s="6">
+      <c r="S7" s="4">
+        <v>3</v>
+      </c>
+      <c r="T7" s="4">
+        <f>MAX(Q7:S7)</f>
+        <v>3</v>
+      </c>
+      <c r="U7" s="4"/>
+      <c r="V7" s="4">
+        <v>0.38</v>
+      </c>
+      <c r="W7" s="4">
+        <v>0.39</v>
+      </c>
+      <c r="X7" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A8" s="14"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="16"/>
+      <c r="R8" s="16"/>
+      <c r="S8" s="16"/>
+      <c r="T8" s="16"/>
+      <c r="U8" s="16"/>
+      <c r="V8" s="17"/>
+      <c r="W8" s="17"/>
+      <c r="X8" s="17"/>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="2">
+        <v>2</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2">
+        <v>2500</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="4">
+        <v>4374.0965999999999</v>
+      </c>
+      <c r="H9" s="4">
+        <v>4696.6341000000002</v>
+      </c>
+      <c r="I9" s="4">
+        <v>3590.9475499999999</v>
+      </c>
+      <c r="J9" s="4">
+        <f>MIN(G9:I9)</f>
+        <v>3590.9475499999999</v>
+      </c>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4">
+        <v>2684.6662000000001</v>
+      </c>
+      <c r="M9" s="4">
+        <v>2179.9955</v>
+      </c>
+      <c r="N9" s="4">
+        <v>2002.1464000000001</v>
+      </c>
+      <c r="O9" s="4">
+        <f>MIN(L9:N9)</f>
+        <v>2002.1464000000001</v>
+      </c>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4">
+        <v>1.6292</v>
+      </c>
+      <c r="R9" s="4">
+        <v>2.1543999999999999</v>
+      </c>
+      <c r="S9" s="4">
+        <v>1.7935399999999999</v>
+      </c>
+      <c r="T9" s="4">
+        <f>MAX(Q9:S9)</f>
+        <v>2.1543999999999999</v>
+      </c>
+      <c r="U9" s="4"/>
+      <c r="V9" s="4">
+        <v>0.81399999999999995</v>
+      </c>
+      <c r="W9" s="4">
+        <v>1.0771999999999999</v>
+      </c>
+      <c r="X9" s="4">
+        <v>0.89670000000000005</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="2">
+        <v>3</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4">
+        <v>1807.8657499999999</v>
+      </c>
+      <c r="M10" s="4">
+        <v>1690.68265</v>
+      </c>
+      <c r="N10" s="4">
+        <v>1474.0976499999999</v>
+      </c>
+      <c r="O10" s="4">
+        <f t="shared" ref="O10:O13" si="1">MIN(L10:N10)</f>
+        <v>1474.0976499999999</v>
+      </c>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4">
+        <v>2.4194</v>
+      </c>
+      <c r="R10" s="4">
+        <v>2.7770000000000001</v>
+      </c>
+      <c r="S10" s="4">
+        <v>2.4359999999999999</v>
+      </c>
+      <c r="T10" s="4">
+        <f t="shared" ref="T10:T13" si="2">MAX(Q10:S10)</f>
+        <v>2.7770000000000001</v>
+      </c>
+      <c r="U10" s="4"/>
+      <c r="V10" s="4">
+        <v>0.80600000000000005</v>
+      </c>
+      <c r="W10" s="4">
+        <v>0.92598377347753702</v>
+      </c>
+      <c r="X10" s="4">
+        <v>0.81200000000000006</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="2">
+        <v>4</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4">
+        <v>1554.473</v>
+      </c>
+      <c r="M11" s="4">
+        <v>1562.6601499999999</v>
+      </c>
+      <c r="N11" s="4">
+        <v>1172.1104499999999</v>
+      </c>
+      <c r="O11" s="4">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="R7" s="6">
-        <v>0.38</v>
-      </c>
-      <c r="S7" s="6">
-        <v>0.39</v>
-      </c>
-      <c r="T7" s="6">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="3"/>
-      <c r="R8" s="3"/>
-      <c r="S8" s="3"/>
-      <c r="T8" s="3"/>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="3">
+        <v>1172.1104499999999</v>
+      </c>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4">
+        <v>2.8130000000000002</v>
+      </c>
+      <c r="R11" s="4">
+        <v>3.0055369999999999</v>
+      </c>
+      <c r="S11" s="4">
+        <v>3.0630000000000002</v>
+      </c>
+      <c r="T11" s="4">
+        <f t="shared" si="2"/>
+        <v>3.0630000000000002</v>
+      </c>
+      <c r="U11" s="4"/>
+      <c r="V11" s="4">
+        <v>0.70299999999999996</v>
+      </c>
+      <c r="W11" s="4">
+        <v>0.75138444210022304</v>
+      </c>
+      <c r="X11" s="4">
+        <v>0.76500000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="2">
+        <v>5</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4">
+        <v>1371.6228000000001</v>
+      </c>
+      <c r="M12" s="5">
+        <v>1409.3516999999999</v>
+      </c>
+      <c r="N12" s="4">
+        <v>1119.4682499999999</v>
+      </c>
+      <c r="O12" s="4">
+        <f t="shared" si="1"/>
+        <v>1119.4682499999999</v>
+      </c>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4">
+        <v>3.1880000000000002</v>
+      </c>
+      <c r="R12" s="4">
+        <v>3.3323999999999998</v>
+      </c>
+      <c r="S12" s="4">
+        <v>3.2069999999999999</v>
+      </c>
+      <c r="T12" s="4">
+        <f t="shared" si="2"/>
+        <v>3.3323999999999998</v>
+      </c>
+      <c r="U12" s="4"/>
+      <c r="V12" s="4">
+        <v>0.63779875925072205</v>
+      </c>
+      <c r="W12" s="4">
+        <v>0.66649568024787498</v>
+      </c>
+      <c r="X12" s="4">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="2">
+        <v>6</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4">
+        <v>1296.1840999999999</v>
+      </c>
+      <c r="M13" s="4">
+        <v>1491.4474</v>
+      </c>
+      <c r="N13" s="4">
+        <v>1210.6604</v>
+      </c>
+      <c r="O13" s="4">
+        <f t="shared" si="1"/>
+        <v>1210.6604</v>
+      </c>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4">
+        <v>3.37459</v>
+      </c>
+      <c r="R13" s="4">
+        <v>3.149</v>
+      </c>
+      <c r="S13" s="4">
+        <v>2.9661</v>
+      </c>
+      <c r="T13" s="4">
+        <f t="shared" si="2"/>
+        <v>3.37459</v>
+      </c>
+      <c r="U13" s="4"/>
+      <c r="V13" s="4">
+        <v>0.56243252791019505</v>
+      </c>
+      <c r="W13" s="4">
+        <v>0.52484073524818897</v>
+      </c>
+      <c r="X13" s="4">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
+      <c r="V14" s="2"/>
+      <c r="W14" s="2"/>
+      <c r="X14" s="2"/>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="2">
         <v>2</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3">
-        <v>2500</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="3"/>
-      <c r="R9" s="3"/>
-      <c r="S9" s="3"/>
-      <c r="T9" s="3"/>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="3">
-        <v>3</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
-      <c r="R10" s="3"/>
-      <c r="S10" s="3"/>
-      <c r="T10" s="3"/>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="3">
+      <c r="C15" s="2"/>
+      <c r="D15" s="2">
+        <v>3500</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="G15" s="4">
+        <v>7886.9699000000001</v>
+      </c>
+      <c r="H15" s="5">
+        <v>7189.9579999999996</v>
+      </c>
+      <c r="I15" s="4">
+        <v>6946.7186499999998</v>
+      </c>
+      <c r="J15" s="4">
+        <f>MIN(G15:I15)</f>
+        <v>6946.7186499999998</v>
+      </c>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4">
+        <v>4704.8050999999996</v>
+      </c>
+      <c r="M15" s="4">
+        <v>4237.4497499999998</v>
+      </c>
+      <c r="N15" s="4">
+        <v>3579.0030499999998</v>
+      </c>
+      <c r="O15" s="4">
+        <f>MIN(L15:N15)</f>
+        <v>3579.0030499999998</v>
+      </c>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="4"/>
+      <c r="R15" s="4"/>
+      <c r="S15" s="4"/>
+      <c r="T15" s="4"/>
+      <c r="U15" s="4"/>
+      <c r="V15" s="4"/>
+      <c r="W15" s="4"/>
+      <c r="X15" s="4"/>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="2">
+        <v>3</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4">
+        <v>3344.6293500000002</v>
+      </c>
+      <c r="M16" s="4">
+        <v>3209.5850999999998</v>
+      </c>
+      <c r="N16" s="4">
+        <v>2735.3495499999999</v>
+      </c>
+      <c r="O16" s="4">
+        <f t="shared" ref="O16:O19" si="3">MIN(L16:N16)</f>
+        <v>2735.3495499999999</v>
+      </c>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="4"/>
+      <c r="R16" s="4"/>
+      <c r="S16" s="4"/>
+      <c r="T16" s="4"/>
+      <c r="U16" s="4"/>
+      <c r="V16" s="4"/>
+      <c r="W16" s="4"/>
+      <c r="X16" s="4"/>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="2">
         <v>4</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="3"/>
-      <c r="R11" s="3"/>
-      <c r="S11" s="3"/>
-      <c r="T11" s="3"/>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="3">
+      <c r="C17" s="2"/>
+      <c r="D17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4">
+        <v>2754.6887499999998</v>
+      </c>
+      <c r="M17" s="4">
+        <v>3083.3841499999999</v>
+      </c>
+      <c r="N17" s="4">
+        <v>2576.1098000000002</v>
+      </c>
+      <c r="O17" s="4">
+        <f t="shared" si="3"/>
+        <v>2576.1098000000002</v>
+      </c>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="4"/>
+      <c r="R17" s="4"/>
+      <c r="S17" s="4"/>
+      <c r="T17" s="4"/>
+      <c r="U17" s="4"/>
+      <c r="V17" s="4"/>
+      <c r="W17" s="4"/>
+      <c r="X17" s="4"/>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="2">
         <v>5</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="3"/>
-      <c r="R12" s="3"/>
-      <c r="S12" s="3"/>
-      <c r="T12" s="3"/>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="3">
+      <c r="C18" s="2"/>
+      <c r="D18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18" s="2"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4">
+        <v>2446.0747000000001</v>
+      </c>
+      <c r="M18" s="4">
+        <v>2833.7763500000001</v>
+      </c>
+      <c r="N18" s="4">
+        <v>2336.0162999999998</v>
+      </c>
+      <c r="O18" s="4">
+        <f t="shared" si="3"/>
+        <v>2336.0162999999998</v>
+      </c>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="4"/>
+      <c r="R18" s="4"/>
+      <c r="S18" s="4"/>
+      <c r="T18" s="4"/>
+      <c r="U18" s="4"/>
+      <c r="V18" s="4"/>
+      <c r="W18" s="4"/>
+      <c r="X18" s="4"/>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="2">
         <v>6</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
-      <c r="Q13" s="3"/>
-      <c r="R13" s="3"/>
-      <c r="S13" s="3"/>
-      <c r="T13" s="3"/>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
-      <c r="P14" s="3"/>
-      <c r="Q14" s="3"/>
-      <c r="R14" s="3"/>
-      <c r="S14" s="3"/>
-      <c r="T14" s="3"/>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" s="3">
+      <c r="C19" s="2"/>
+      <c r="D19" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F19" s="2"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4">
+        <v>2802.9258</v>
+      </c>
+      <c r="M19" s="4">
+        <v>2744.8560000000002</v>
+      </c>
+      <c r="N19" s="4">
+        <v>2172.9760500000002</v>
+      </c>
+      <c r="O19" s="4">
+        <f t="shared" si="3"/>
+        <v>2172.9760500000002</v>
+      </c>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4"/>
+      <c r="R19" s="4"/>
+      <c r="S19" s="4"/>
+      <c r="T19" s="4"/>
+      <c r="U19" s="4"/>
+      <c r="V19" s="4"/>
+      <c r="W19" s="4"/>
+      <c r="X19" s="4"/>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="2"/>
+      <c r="S20" s="2"/>
+      <c r="T20" s="2"/>
+      <c r="U20" s="2"/>
+      <c r="V20" s="2"/>
+      <c r="W20" s="2"/>
+      <c r="X20" s="2"/>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="2">
         <v>2</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3">
-        <v>3500</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F15" s="3"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
-      <c r="O15" s="3"/>
-      <c r="P15" s="3"/>
-      <c r="Q15" s="3"/>
-      <c r="R15" s="3"/>
-      <c r="S15" s="3"/>
-      <c r="T15" s="3"/>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B16" s="3">
-        <v>3</v>
-      </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
-      <c r="O16" s="3"/>
-      <c r="P16" s="3"/>
-      <c r="Q16" s="3"/>
-      <c r="R16" s="3"/>
-      <c r="S16" s="3"/>
-      <c r="T16" s="3"/>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B17" s="3">
+      <c r="C21" s="2"/>
+      <c r="D21" s="2">
+        <v>5000</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="2"/>
+      <c r="S21" s="2"/>
+      <c r="T21" s="2"/>
+      <c r="U21" s="2"/>
+      <c r="V21" s="2"/>
+      <c r="W21" s="2"/>
+      <c r="X21" s="2"/>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="2">
+        <v>3</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="2"/>
+      <c r="S22" s="2"/>
+      <c r="T22" s="2"/>
+      <c r="U22" s="2"/>
+      <c r="V22" s="2"/>
+      <c r="W22" s="2"/>
+      <c r="X22" s="2"/>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="2">
         <v>4</v>
       </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
-      <c r="P17" s="3"/>
-      <c r="Q17" s="3"/>
-      <c r="R17" s="3"/>
-      <c r="S17" s="3"/>
-      <c r="T17" s="3"/>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B18" s="3">
+      <c r="C23" s="2"/>
+      <c r="D23" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2"/>
+      <c r="S23" s="2"/>
+      <c r="T23" s="2"/>
+      <c r="U23" s="2"/>
+      <c r="V23" s="2"/>
+      <c r="W23" s="2"/>
+      <c r="X23" s="2"/>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="2">
         <v>5</v>
       </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
-      <c r="Q18" s="3"/>
-      <c r="R18" s="3"/>
-      <c r="S18" s="3"/>
-      <c r="T18" s="3"/>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B19" s="3">
+      <c r="C24" s="2"/>
+      <c r="D24" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="2">
         <v>6</v>
       </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
-      <c r="O19" s="3"/>
-      <c r="P19" s="3"/>
-      <c r="Q19" s="3"/>
-      <c r="R19" s="3"/>
-      <c r="S19" s="3"/>
-      <c r="T19" s="3"/>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-      <c r="O20" s="3"/>
-      <c r="P20" s="3"/>
-      <c r="Q20" s="3"/>
-      <c r="R20" s="3"/>
-      <c r="S20" s="3"/>
-      <c r="T20" s="3"/>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B21" s="3">
-        <v>2</v>
-      </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3">
-        <v>5000</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-      <c r="O21" s="3"/>
-      <c r="P21" s="3"/>
-      <c r="Q21" s="3"/>
-      <c r="R21" s="3"/>
-      <c r="S21" s="3"/>
-      <c r="T21" s="3"/>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B22" s="3">
-        <v>3</v>
-      </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
-      <c r="O22" s="3"/>
-      <c r="P22" s="3"/>
-      <c r="Q22" s="3"/>
-      <c r="R22" s="3"/>
-      <c r="S22" s="3"/>
-      <c r="T22" s="3"/>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B23" s="3">
-        <v>4</v>
-      </c>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
-      <c r="N23" s="3"/>
-      <c r="O23" s="3"/>
-      <c r="P23" s="3"/>
-      <c r="Q23" s="3"/>
-      <c r="R23" s="3"/>
-      <c r="S23" s="3"/>
-      <c r="T23" s="3"/>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B24" s="3">
-        <v>5</v>
-      </c>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B25" s="3">
-        <v>6</v>
-      </c>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F25" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="A1:X1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Working on results documentation
</commit_message>
<xml_diff>
--- a/PerformanceTable.xlsx
+++ b/PerformanceTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Project Files\N-Body\Parallel-N-Body\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AC8327D-84C3-4BAF-9720-BE5208FCF8D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{459941D8-D73B-4B95-B465-0D3E3E6D3D23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{7E97CE3A-31D6-4C49-8965-2B1756764954}"/>
   </bookViews>
@@ -1089,7 +1089,7 @@
   <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N32" sqref="N32"/>
+      <selection activeCell="U23" sqref="U23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -2329,9 +2329,15 @@
         <v>4.05796399144144</v>
       </c>
       <c r="P25" s="2"/>
-      <c r="Q25" s="2"/>
-      <c r="R25" s="2"/>
-      <c r="S25" s="2"/>
+      <c r="Q25" s="2">
+        <v>1.0400908449642901</v>
+      </c>
+      <c r="R25" s="2">
+        <v>2.02898199572072</v>
+      </c>
+      <c r="S25" s="2">
+        <v>0.874733921825536</v>
+      </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
@@ -2378,9 +2384,15 @@
         <v>5.2365656024729503</v>
       </c>
       <c r="P26" s="2"/>
-      <c r="Q26" s="2"/>
-      <c r="R26" s="2"/>
-      <c r="S26" s="2"/>
+      <c r="Q26" s="2">
+        <v>0.87382680949817904</v>
+      </c>
+      <c r="R26" s="2">
+        <v>1.74552186749098</v>
+      </c>
+      <c r="S26" s="2">
+        <v>0.65473294332200205</v>
+      </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
@@ -2427,9 +2439,15 @@
         <v>4.9125044689607904</v>
       </c>
       <c r="P27" s="2"/>
-      <c r="Q27" s="2"/>
-      <c r="R27" s="2"/>
-      <c r="S27" s="2"/>
+      <c r="Q27" s="2">
+        <v>0.75470235591996904</v>
+      </c>
+      <c r="R27" s="2">
+        <v>1.2281261172402</v>
+      </c>
+      <c r="S27" s="2">
+        <v>0.638434277152512</v>
+      </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
@@ -2473,6 +2491,15 @@
         <f t="shared" si="6"/>
         <v>4.8746592398217903</v>
       </c>
+      <c r="Q28" s="1">
+        <v>0.69075647124898698</v>
+      </c>
+      <c r="R28" s="1">
+        <v>0.97493184796435794</v>
+      </c>
+      <c r="S28" s="1">
+        <v>0.55125293686424304</v>
+      </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
@@ -2515,6 +2542,15 @@
       <c r="O29" s="2">
         <f t="shared" si="6"/>
         <v>5.1253526212284699</v>
+      </c>
+      <c r="Q29" s="1">
+        <v>0.67437209753178495</v>
+      </c>
+      <c r="R29" s="1">
+        <v>0.85422543687141195</v>
+      </c>
+      <c r="S29" s="1">
+        <v>0.48331781021119702</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">

</xml_diff>